<commit_message>
excel open file birthday
</commit_message>
<xml_diff>
--- a/scr/Книга1.xlsx
+++ b/scr/Книга1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC1\PycharmProjects\CoinGraphics\scr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03FE9A51-5AF6-4413-AB31-08F2FAB12654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA29F0C-9F6D-4906-B3B2-7A308712B0D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1425" windowWidth="21600" windowHeight="11295" xr2:uid="{07E3C363-2872-48BA-909D-E6ECE8DDAFBD}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{07E3C363-2872-48BA-909D-E6ECE8DDAFBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="78">
   <si>
     <t>№</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Быстрицкий Глеб Валентинович</t>
-  </si>
-  <si>
-    <t>28.01.0201</t>
   </si>
   <si>
     <t>Быстрицкая Анна Константиновна, asemenova077@gmail.com</t>
@@ -627,7 +624,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,14 +884,14 @@
       <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1">
+        <v>44224</v>
+      </c>
+      <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
@@ -903,10 +900,10 @@
         <v>13</v>
       </c>
       <c r="H10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" t="s">
         <v>49</v>
-      </c>
-      <c r="I10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -914,16 +911,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1">
         <v>40482</v>
       </c>
       <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
         <v>52</v>
-      </c>
-      <c r="E11" t="s">
-        <v>53</v>
       </c>
       <c r="F11" t="s">
         <v>12</v>
@@ -934,16 +931,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1">
         <v>39587</v>
       </c>
       <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
         <v>55</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
       </c>
       <c r="F12" t="s">
         <v>12</v>
@@ -952,10 +949,10 @@
         <v>13</v>
       </c>
       <c r="H12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" t="s">
         <v>57</v>
-      </c>
-      <c r="I12" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -963,7 +960,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1">
         <v>40753</v>
@@ -975,10 +972,10 @@
         <v>13</v>
       </c>
       <c r="H13" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" t="s">
         <v>60</v>
-      </c>
-      <c r="I13" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -986,25 +983,25 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1">
         <v>39414</v>
       </c>
       <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
         <v>63</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" t="s">
         <v>64</v>
       </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>65</v>
-      </c>
-      <c r="I14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1012,13 +1009,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="1">
         <v>39269</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15">
         <v>89520299983</v>
@@ -1030,10 +1027,10 @@
         <v>13</v>
       </c>
       <c r="H15" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" t="s">
         <v>69</v>
-      </c>
-      <c r="I15" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1041,16 +1038,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="1">
         <v>39002</v>
       </c>
       <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" t="s">
         <v>72</v>
-      </c>
-      <c r="H16" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1058,25 +1055,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="1">
         <v>40282</v>
       </c>
       <c r="D17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
         <v>75</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
         <v>76</v>
       </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>77</v>
-      </c>
-      <c r="I17" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>